<commit_message>
Updated filepaths for stat testing
</commit_message>
<xml_diff>
--- a/Stat_Filepaths.xlsx
+++ b/Stat_Filepaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/tom/Rectal Segmentation/Data-MultipleExperts/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD788340-0EBA-8741-99FC-152BE5BD2BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDDB48D-0D0F-E34C-81DD-7FC02A6CE47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="60160" windowHeight="33840" xr2:uid="{B771CA73-2591-9C46-8A47-23A52B587D94}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="60160" windowHeight="31660" xr2:uid="{B771CA73-2591-9C46-8A47-23A52B587D94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,10 +504,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>